<commit_message>
updated excel and selecting only our groups data
</commit_message>
<xml_diff>
--- a/data for each group_2025.xlsx
+++ b/data for each group_2025.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29602"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ugentbe-my.sharepoint.com/personal/junwei_hu_ugent_be/Documents/桌面/GENT RESEARCHT/appied soil biology/2024 soil biology/practical materials/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\colby\Documents\R\Soil_Biology\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="480" documentId="11_F25DC773A252ABDACC1048D3A19D695C5ADE58EA" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{98C86D87-14A7-4A59-A0CE-492F560C6159}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBB2C77A-9DDD-4371-A9A8-313BD9FDD6D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-16200" yWindow="-13068" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -80,10 +80,9 @@
   <authors>
     <author>tc={5F75FB8B-FAEF-40E0-9FE5-463021C6A2AD}</author>
     <author>tc={A9C199A3-A269-44F2-93A5-2FF8E34BDA83}</author>
-    <author>tc={6226B021-851D-4AA5-A6DD-C2CE5C268F52}</author>
   </authors>
   <commentList>
-    <comment ref="L2" authorId="0" shapeId="0" xr:uid="{5F75FB8B-FAEF-40E0-9FE5-463021C6A2AD}">
+    <comment ref="I2" authorId="0" shapeId="0" xr:uid="{5F75FB8B-FAEF-40E0-9FE5-463021C6A2AD}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -91,7 +90,7 @@
     shouldnt it be m^3?</t>
       </text>
     </comment>
-    <comment ref="S2" authorId="1" shapeId="0" xr:uid="{A9C199A3-A269-44F2-93A5-2FF8E34BDA83}">
+    <comment ref="M2" authorId="1" shapeId="0" xr:uid="{A9C199A3-A269-44F2-93A5-2FF8E34BDA83}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -99,22 +98,12 @@
     assume soil core is 5cm diameter and 5cm depth</t>
       </text>
     </comment>
-    <comment ref="AK2" authorId="2" shapeId="0" xr:uid="{6226B021-851D-4AA5-A6DD-C2CE5C268F52}">
-      <text>
-        <t xml:space="preserve">[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    according to protocol
-Reply:
-    Practical 2/3 </t>
-      </text>
-    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="93">
   <si>
     <t>plot</t>
   </si>
@@ -392,7 +381,7 @@
     <t>U</t>
   </si>
   <si>
-    <t>mass fresh soil (g)</t>
+    <t>landuse</t>
   </si>
 </sst>
 </file>
@@ -405,7 +394,7 @@
     <numFmt numFmtId="166" formatCode="0.0"/>
     <numFmt numFmtId="167" formatCode="0.000"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -432,6 +421,7 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -485,7 +475,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -522,11 +512,12 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -830,17 +821,11 @@
 
 <file path=xl/threadedComments/threadedComment2.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="L2" dT="2025-12-08T12:43:55.08" personId="{7437451D-0B66-4ED4-A305-06D7E3BFFEAC}" id="{5F75FB8B-FAEF-40E0-9FE5-463021C6A2AD}">
+  <threadedComment ref="I2" dT="2025-12-08T12:43:55.08" personId="{7437451D-0B66-4ED4-A305-06D7E3BFFEAC}" id="{5F75FB8B-FAEF-40E0-9FE5-463021C6A2AD}">
     <text>shouldnt it be m^3?</text>
   </threadedComment>
-  <threadedComment ref="S2" dT="2025-12-08T13:00:41.14" personId="{7437451D-0B66-4ED4-A305-06D7E3BFFEAC}" id="{A9C199A3-A269-44F2-93A5-2FF8E34BDA83}">
+  <threadedComment ref="M2" dT="2025-12-08T13:00:41.14" personId="{7437451D-0B66-4ED4-A305-06D7E3BFFEAC}" id="{A9C199A3-A269-44F2-93A5-2FF8E34BDA83}">
     <text>assume soil core is 5cm diameter and 5cm depth</text>
-  </threadedComment>
-  <threadedComment ref="AK2" dT="2025-12-08T12:51:06.86" personId="{7437451D-0B66-4ED4-A305-06D7E3BFFEAC}" id="{6226B021-851D-4AA5-A6DD-C2CE5C268F52}">
-    <text>according to protocol</text>
-  </threadedComment>
-  <threadedComment ref="AK2" dT="2025-12-08T13:11:00.75" personId="{7437451D-0B66-4ED4-A305-06D7E3BFFEAC}" id="{F887F983-A558-4866-B517-2EF26DF728BD}" parentId="{6226B021-851D-4AA5-A6DD-C2CE5C268F52}">
-    <text xml:space="preserve">Practical 2/3 </text>
   </threadedComment>
 </ThreadedComments>
 </file>
@@ -853,64 +838,64 @@
       <selection activeCell="AH4" sqref="AH4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="8" max="9" width="15" customWidth="1"/>
-    <col min="10" max="11" width="13.5703125" customWidth="1"/>
+    <col min="10" max="11" width="13.5546875" customWidth="1"/>
     <col min="12" max="13" width="13" customWidth="1"/>
-    <col min="14" max="15" width="15.28515625" customWidth="1"/>
-    <col min="16" max="17" width="14.85546875" customWidth="1"/>
-    <col min="18" max="18" width="12.7109375" customWidth="1"/>
-    <col min="19" max="20" width="15.7109375" customWidth="1"/>
-    <col min="21" max="22" width="11.42578125" customWidth="1"/>
-    <col min="23" max="24" width="13.28515625" customWidth="1"/>
+    <col min="14" max="15" width="15.33203125" customWidth="1"/>
+    <col min="16" max="17" width="14.88671875" customWidth="1"/>
+    <col min="18" max="18" width="12.6640625" customWidth="1"/>
+    <col min="19" max="20" width="15.6640625" customWidth="1"/>
+    <col min="21" max="22" width="11.44140625" customWidth="1"/>
+    <col min="23" max="24" width="13.33203125" customWidth="1"/>
     <col min="25" max="26" width="15" customWidth="1"/>
-    <col min="27" max="28" width="16.28515625" customWidth="1"/>
-    <col min="29" max="30" width="14.7109375" customWidth="1"/>
-    <col min="31" max="31" width="10.28515625" customWidth="1"/>
-    <col min="32" max="36" width="10.7109375" customWidth="1"/>
+    <col min="27" max="28" width="16.33203125" customWidth="1"/>
+    <col min="29" max="30" width="14.6640625" customWidth="1"/>
+    <col min="31" max="31" width="10.33203125" customWidth="1"/>
+    <col min="32" max="36" width="10.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" ht="39" customHeight="1">
-      <c r="A1" s="24" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="24" t="s">
+    <row r="1" spans="1:37" ht="39" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="24" t="s">
+      <c r="C1" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="24" t="s">
+      <c r="D1" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
-      <c r="K1" s="24"/>
-      <c r="L1" s="23" t="s">
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
+      <c r="K1" s="23"/>
+      <c r="L1" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="M1" s="23"/>
-      <c r="N1" s="23"/>
+      <c r="M1" s="24"/>
+      <c r="N1" s="24"/>
       <c r="O1" s="5"/>
-      <c r="P1" s="24" t="s">
+      <c r="P1" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="Q1" s="24"/>
-      <c r="R1" s="24"/>
-      <c r="S1" s="23" t="s">
+      <c r="Q1" s="23"/>
+      <c r="R1" s="23"/>
+      <c r="S1" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="T1" s="23"/>
-      <c r="U1" s="23"/>
-      <c r="V1" s="23"/>
-      <c r="W1" s="23"/>
-      <c r="X1" s="23"/>
-      <c r="Y1" s="23"/>
+      <c r="T1" s="24"/>
+      <c r="U1" s="24"/>
+      <c r="V1" s="24"/>
+      <c r="W1" s="24"/>
+      <c r="X1" s="24"/>
+      <c r="Y1" s="24"/>
       <c r="Z1" s="5"/>
       <c r="AA1" t="s">
         <v>7</v>
@@ -919,19 +904,19 @@
         <v>8</v>
       </c>
       <c r="AD1" s="6"/>
-      <c r="AE1" s="23" t="s">
+      <c r="AE1" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="AF1" s="23"/>
-      <c r="AG1" s="23"/>
-      <c r="AH1" s="23"/>
-      <c r="AI1" s="23"/>
-      <c r="AJ1" s="23"/>
-    </row>
-    <row r="2" spans="1:37" ht="81.599999999999994" customHeight="1">
-      <c r="A2" s="24"/>
-      <c r="B2" s="24"/>
-      <c r="C2" s="24"/>
+      <c r="AF1" s="24"/>
+      <c r="AG1" s="24"/>
+      <c r="AH1" s="24"/>
+      <c r="AI1" s="24"/>
+      <c r="AJ1" s="24"/>
+    </row>
+    <row r="2" spans="1:37" ht="81.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="23"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
       <c r="D2" s="6" t="s">
         <v>10</v>
       </c>
@@ -1033,7 +1018,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:37" s="3" customFormat="1">
+    <row r="3" spans="1:37" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A3" s="8">
         <v>1</v>
       </c>
@@ -1147,7 +1132,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:37" s="3" customFormat="1">
+    <row r="4" spans="1:37" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A4" s="8">
         <v>2</v>
       </c>
@@ -1258,7 +1243,7 @@
       <c r="AJ4" s="10"/>
       <c r="AK4" s="8"/>
     </row>
-    <row r="5" spans="1:37" s="3" customFormat="1">
+    <row r="5" spans="1:37" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A5" s="8">
         <v>3</v>
       </c>
@@ -1369,7 +1354,7 @@
       <c r="AJ5" s="10"/>
       <c r="AK5" s="8"/>
     </row>
-    <row r="6" spans="1:37" s="3" customFormat="1">
+    <row r="6" spans="1:37" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A6" s="8">
         <v>4</v>
       </c>
@@ -1480,7 +1465,7 @@
       <c r="AJ6" s="10"/>
       <c r="AK6" s="8"/>
     </row>
-    <row r="7" spans="1:37" s="3" customFormat="1">
+    <row r="7" spans="1:37" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A7" s="8">
         <v>5</v>
       </c>
@@ -1591,7 +1576,7 @@
       <c r="AJ7" s="10"/>
       <c r="AK7" s="8"/>
     </row>
-    <row r="8" spans="1:37" s="3" customFormat="1">
+    <row r="8" spans="1:37" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A8" s="8">
         <v>6</v>
       </c>
@@ -1702,7 +1687,7 @@
       <c r="AJ8" s="10"/>
       <c r="AK8" s="8"/>
     </row>
-    <row r="9" spans="1:37" s="3" customFormat="1">
+    <row r="9" spans="1:37" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A9" s="8">
         <v>7</v>
       </c>
@@ -1813,7 +1798,7 @@
       <c r="AJ9" s="10"/>
       <c r="AK9" s="8"/>
     </row>
-    <row r="10" spans="1:37" s="3" customFormat="1">
+    <row r="10" spans="1:37" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A10" s="8">
         <v>8</v>
       </c>
@@ -1924,7 +1909,7 @@
       <c r="AJ10" s="10"/>
       <c r="AK10" s="8"/>
     </row>
-    <row r="11" spans="1:37" s="3" customFormat="1">
+    <row r="11" spans="1:37" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A11" s="8">
         <v>9</v>
       </c>
@@ -2035,7 +2020,7 @@
       <c r="AJ11" s="10"/>
       <c r="AK11" s="8"/>
     </row>
-    <row r="12" spans="1:37" s="3" customFormat="1">
+    <row r="12" spans="1:37" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A12" s="8">
         <v>10</v>
       </c>
@@ -2146,7 +2131,7 @@
       <c r="AJ12" s="10"/>
       <c r="AK12" s="8"/>
     </row>
-    <row r="13" spans="1:37" s="3" customFormat="1">
+    <row r="13" spans="1:37" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
         <v>11</v>
       </c>
@@ -2255,7 +2240,7 @@
       <c r="AI13" s="15"/>
       <c r="AJ13" s="15"/>
     </row>
-    <row r="14" spans="1:37" s="3" customFormat="1">
+    <row r="14" spans="1:37" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A14" s="8">
         <v>12</v>
       </c>
@@ -2366,7 +2351,7 @@
       <c r="AJ14" s="10"/>
       <c r="AK14" s="8"/>
     </row>
-    <row r="15" spans="1:37" s="3" customFormat="1">
+    <row r="15" spans="1:37" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A15" s="8">
         <v>13</v>
       </c>
@@ -2477,7 +2462,7 @@
       <c r="AJ15" s="10"/>
       <c r="AK15" s="8"/>
     </row>
-    <row r="16" spans="1:37" s="3" customFormat="1">
+    <row r="16" spans="1:37" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A16" s="8">
         <v>14</v>
       </c>
@@ -2588,7 +2573,7 @@
       <c r="AJ16" s="10"/>
       <c r="AK16" s="8"/>
     </row>
-    <row r="17" spans="1:37" s="3" customFormat="1">
+    <row r="17" spans="1:37" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A17" s="8">
         <v>15</v>
       </c>
@@ -2699,7 +2684,7 @@
       <c r="AJ17" s="10"/>
       <c r="AK17" s="8"/>
     </row>
-    <row r="18" spans="1:37" s="3" customFormat="1">
+    <row r="18" spans="1:37" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A18" s="3">
         <v>16</v>
       </c>
@@ -2799,7 +2784,7 @@
       <c r="AI18" s="15"/>
       <c r="AJ18" s="15"/>
     </row>
-    <row r="19" spans="1:37" s="3" customFormat="1">
+    <row r="19" spans="1:37" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A19" s="3">
         <v>17</v>
       </c>
@@ -2899,7 +2884,7 @@
       <c r="AI19" s="15"/>
       <c r="AJ19" s="15"/>
     </row>
-    <row r="20" spans="1:37" s="3" customFormat="1">
+    <row r="20" spans="1:37" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A20" s="3">
         <v>18</v>
       </c>
@@ -2999,7 +2984,7 @@
       <c r="AI20" s="15"/>
       <c r="AJ20" s="15"/>
     </row>
-    <row r="21" spans="1:37" s="3" customFormat="1">
+    <row r="21" spans="1:37" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A21" s="3">
         <v>19</v>
       </c>
@@ -3099,7 +3084,7 @@
       <c r="AI21" s="15"/>
       <c r="AJ21" s="15"/>
     </row>
-    <row r="22" spans="1:37" s="3" customFormat="1">
+    <row r="22" spans="1:37" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A22" s="3">
         <v>20</v>
       </c>
@@ -3199,7 +3184,7 @@
       <c r="AI22" s="15"/>
       <c r="AJ22" s="15"/>
     </row>
-    <row r="23" spans="1:37" s="3" customFormat="1">
+    <row r="23" spans="1:37" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A23" s="3">
         <v>21</v>
       </c>
@@ -3299,7 +3284,7 @@
       <c r="AI23" s="15"/>
       <c r="AJ23" s="15"/>
     </row>
-    <row r="24" spans="1:37" s="3" customFormat="1">
+    <row r="24" spans="1:37" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A24" s="3">
         <v>22</v>
       </c>
@@ -3399,7 +3384,7 @@
       <c r="AI24" s="15"/>
       <c r="AJ24" s="15"/>
     </row>
-    <row r="25" spans="1:37" s="3" customFormat="1">
+    <row r="25" spans="1:37" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A25" s="3">
         <v>23</v>
       </c>
@@ -3499,29 +3484,29 @@
       <c r="AI25" s="15"/>
       <c r="AJ25" s="15"/>
     </row>
-    <row r="26" spans="1:37" ht="50.45" customHeight="1">
-      <c r="D26" s="23"/>
-      <c r="E26" s="23"/>
+    <row r="26" spans="1:37" ht="50.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D26" s="24"/>
+      <c r="E26" s="24"/>
       <c r="J26" s="6"/>
       <c r="K26" s="6"/>
-      <c r="L26" s="24"/>
-      <c r="M26" s="24"/>
-      <c r="N26" s="24"/>
+      <c r="L26" s="23"/>
+      <c r="M26" s="23"/>
+      <c r="N26" s="23"/>
       <c r="O26" s="4"/>
-      <c r="S26" s="24"/>
-      <c r="T26" s="24"/>
-      <c r="U26" s="24"/>
-      <c r="V26" s="24"/>
-      <c r="W26" s="24"/>
-      <c r="X26" s="24"/>
-      <c r="Y26" s="24"/>
+      <c r="S26" s="23"/>
+      <c r="T26" s="23"/>
+      <c r="U26" s="23"/>
+      <c r="V26" s="23"/>
+      <c r="W26" s="23"/>
+      <c r="X26" s="23"/>
+      <c r="Y26" s="23"/>
       <c r="Z26" s="4"/>
       <c r="AA26" s="5"/>
       <c r="AB26" s="5"/>
       <c r="AC26" s="6"/>
       <c r="AD26" s="6"/>
-      <c r="AE26" s="23"/>
-      <c r="AF26" s="23"/>
+      <c r="AE26" s="24"/>
+      <c r="AF26" s="24"/>
       <c r="AG26" s="5"/>
       <c r="AH26" s="5"/>
       <c r="AI26" s="5"/>
@@ -3529,11 +3514,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="L1:N1"/>
-    <mergeCell ref="D1:K1"/>
     <mergeCell ref="S1:Y1"/>
     <mergeCell ref="D26:E26"/>
     <mergeCell ref="L26:N26"/>
@@ -3541,6 +3521,11 @@
     <mergeCell ref="AE26:AF26"/>
     <mergeCell ref="P1:R1"/>
     <mergeCell ref="AE1:AJ1"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="L1:N1"/>
+    <mergeCell ref="D1:K1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -3555,16 +3540,16 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="22.28515625" customWidth="1"/>
-    <col min="4" max="4" width="21.42578125" customWidth="1"/>
-    <col min="5" max="5" width="20.7109375" customWidth="1"/>
-    <col min="6" max="6" width="14.7109375" customWidth="1"/>
-    <col min="7" max="7" width="16.140625" customWidth="1"/>
+    <col min="3" max="3" width="22.33203125" customWidth="1"/>
+    <col min="4" max="4" width="21.44140625" customWidth="1"/>
+    <col min="5" max="5" width="20.6640625" customWidth="1"/>
+    <col min="6" max="6" width="14.6640625" customWidth="1"/>
+    <col min="7" max="7" width="16.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>45</v>
       </c>
@@ -3587,7 +3572,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:7" hidden="1">
+    <row r="2" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>52</v>
       </c>
@@ -3604,7 +3589,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="3" spans="1:7" hidden="1">
+    <row r="3" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>56</v>
       </c>
@@ -3621,7 +3606,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="4" spans="1:7" hidden="1">
+    <row r="4" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>58</v>
       </c>
@@ -3638,7 +3623,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="5" spans="1:7" hidden="1">
+    <row r="5" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>60</v>
       </c>
@@ -3655,7 +3640,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="6" spans="1:7" hidden="1">
+    <row r="6" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>61</v>
       </c>
@@ -3672,7 +3657,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>63</v>
       </c>
@@ -3689,7 +3674,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="8" spans="1:7" hidden="1">
+    <row r="8" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>66</v>
       </c>
@@ -3706,7 +3691,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="9" spans="1:7" hidden="1">
+    <row r="9" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>70</v>
       </c>
@@ -3723,7 +3708,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="10" spans="1:7" hidden="1">
+    <row r="10" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>73</v>
       </c>
@@ -3740,7 +3725,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="11" spans="1:7" hidden="1">
+    <row r="11" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>76</v>
       </c>
@@ -3757,7 +3742,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="12" spans="1:7" hidden="1">
+    <row r="12" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>78</v>
       </c>
@@ -3774,7 +3759,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="13" spans="1:7" hidden="1">
+    <row r="13" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>79</v>
       </c>
@@ -3791,7 +3776,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="14" spans="1:7" hidden="1">
+    <row r="14" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>81</v>
       </c>
@@ -3808,7 +3793,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="15" spans="1:7" hidden="1">
+    <row r="15" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>82</v>
       </c>
@@ -3825,7 +3810,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="16" spans="1:7" hidden="1">
+    <row r="16" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>83</v>
       </c>
@@ -3842,7 +3827,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="17" spans="1:5" hidden="1">
+    <row r="17" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>84</v>
       </c>
@@ -3859,7 +3844,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="18" spans="1:5" hidden="1">
+    <row r="18" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>85</v>
       </c>
@@ -3876,7 +3861,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="19" spans="1:5" hidden="1">
+    <row r="19" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>87</v>
       </c>
@@ -3893,7 +3878,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="20" spans="1:5" hidden="1">
+    <row r="20" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>88</v>
       </c>
@@ -3910,7 +3895,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="21" spans="1:5" hidden="1">
+    <row r="21" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>89</v>
       </c>
@@ -3927,7 +3912,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="22" spans="1:5" hidden="1">
+    <row r="22" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>91</v>
       </c>
@@ -3952,193 +3937,126 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04687CA9-6388-4DB5-AAB6-91A2B64027C2}">
-  <dimension ref="A1:AK26"/>
+  <dimension ref="A1:T26"/>
   <sheetViews>
-    <sheetView topLeftCell="V1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="AK3" sqref="AK3"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="8" max="9" width="15" customWidth="1"/>
-    <col min="10" max="11" width="13.5703125" customWidth="1"/>
-    <col min="12" max="13" width="13" customWidth="1"/>
-    <col min="14" max="15" width="15.28515625" customWidth="1"/>
-    <col min="16" max="17" width="14.85546875" customWidth="1"/>
-    <col min="18" max="18" width="12.7109375" customWidth="1"/>
-    <col min="19" max="20" width="15.7109375" customWidth="1"/>
-    <col min="21" max="22" width="11.42578125" customWidth="1"/>
-    <col min="23" max="24" width="13.28515625" customWidth="1"/>
-    <col min="25" max="26" width="15" customWidth="1"/>
-    <col min="27" max="28" width="16.28515625" customWidth="1"/>
-    <col min="29" max="30" width="14.7109375" customWidth="1"/>
-    <col min="31" max="31" width="10.28515625" customWidth="1"/>
-    <col min="32" max="36" width="10.7109375" customWidth="1"/>
+    <col min="7" max="7" width="15" customWidth="1"/>
+    <col min="8" max="8" width="13.5546875" customWidth="1"/>
+    <col min="9" max="9" width="13" customWidth="1"/>
+    <col min="10" max="10" width="15.33203125" customWidth="1"/>
+    <col min="11" max="11" width="14.88671875" customWidth="1"/>
+    <col min="12" max="12" width="12.6640625" customWidth="1"/>
+    <col min="13" max="13" width="15.6640625" customWidth="1"/>
+    <col min="14" max="14" width="11.44140625" customWidth="1"/>
+    <col min="15" max="15" width="13.33203125" customWidth="1"/>
+    <col min="16" max="16" width="15" customWidth="1"/>
+    <col min="17" max="17" width="16.33203125" customWidth="1"/>
+    <col min="18" max="18" width="14.6640625" customWidth="1"/>
+    <col min="19" max="19" width="10.33203125" customWidth="1"/>
+    <col min="20" max="20" width="10.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" ht="39" customHeight="1">
-      <c r="A1" s="24" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="24" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="24" t="s">
+    <row r="1" spans="1:20" ht="39" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D1" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="24" t="s">
+        <v>4</v>
+      </c>
+      <c r="J1" s="24"/>
+      <c r="K1" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="L1" s="23"/>
+      <c r="M1" s="24" t="s">
+        <v>6</v>
+      </c>
+      <c r="N1" s="24"/>
+      <c r="O1" s="24"/>
+      <c r="P1" s="24"/>
+      <c r="Q1" t="s">
+        <v>7</v>
+      </c>
+      <c r="R1" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="S1" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="T1" s="24"/>
+    </row>
+    <row r="2" spans="1:20" ht="81.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="25" t="s">
+        <v>92</v>
+      </c>
+      <c r="C2" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="24" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
-      <c r="K1" s="24"/>
-      <c r="L1" s="23" t="s">
-        <v>4</v>
-      </c>
-      <c r="M1" s="23"/>
-      <c r="N1" s="23"/>
-      <c r="O1" s="5"/>
-      <c r="P1" s="24" t="s">
-        <v>5</v>
-      </c>
-      <c r="Q1" s="24"/>
-      <c r="R1" s="24"/>
-      <c r="S1" s="23" t="s">
-        <v>6</v>
-      </c>
-      <c r="T1" s="23"/>
-      <c r="U1" s="23"/>
-      <c r="V1" s="23"/>
-      <c r="W1" s="23"/>
-      <c r="X1" s="23"/>
-      <c r="Y1" s="23"/>
-      <c r="Z1" s="5"/>
-      <c r="AA1" t="s">
-        <v>7</v>
-      </c>
-      <c r="AC1" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="AD1" s="6"/>
-      <c r="AE1" s="23" t="s">
-        <v>9</v>
-      </c>
-      <c r="AF1" s="23"/>
-      <c r="AG1" s="23"/>
-      <c r="AH1" s="23"/>
-      <c r="AI1" s="23"/>
-      <c r="AJ1" s="23"/>
-    </row>
-    <row r="2" spans="1:37" ht="81.599999999999994" customHeight="1">
-      <c r="A2" s="24"/>
-      <c r="B2" s="24"/>
-      <c r="C2" s="24"/>
       <c r="D2" s="6" t="s">
         <v>10</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="7" t="s">
-        <v>12</v>
+      <c r="F2" s="6" t="s">
+        <v>13</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="I2" s="7" t="s">
-        <v>15</v>
+        <v>16</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>18</v>
       </c>
       <c r="J2" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="K2" s="7" t="s">
-        <v>17</v>
+        <v>20</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>22</v>
       </c>
       <c r="L2" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="M2" s="7" t="s">
-        <v>19</v>
+        <v>23</v>
+      </c>
+      <c r="M2" s="6" t="s">
+        <v>24</v>
       </c>
       <c r="N2" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="O2" s="7" t="s">
-        <v>21</v>
+        <v>26</v>
+      </c>
+      <c r="O2" s="6" t="s">
+        <v>28</v>
       </c>
       <c r="P2" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q2" s="7" t="s">
-        <v>22</v>
+        <v>30</v>
+      </c>
+      <c r="Q2" s="6" t="s">
+        <v>32</v>
       </c>
       <c r="R2" s="6" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="S2" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="T2" s="20" t="s">
-        <v>25</v>
-      </c>
-      <c r="U2" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="V2" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="W2" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="X2" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="Y2" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="Z2" s="20" t="s">
-        <v>31</v>
-      </c>
-      <c r="AA2" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="AB2" s="21" t="s">
-        <v>33</v>
-      </c>
-      <c r="AC2" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="AD2" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="AE2" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="AF2" s="6" t="s">
+      <c r="T2" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="AG2" s="7"/>
-      <c r="AH2" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="AI2" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="AJ2" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="AK2" s="19" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="3" spans="1:37" s="3" customFormat="1">
+    </row>
+    <row r="3" spans="1:20" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A3" s="8">
         <v>1</v>
       </c>
@@ -4154,72 +4072,53 @@
       <c r="E3" s="8">
         <v>0.12</v>
       </c>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8">
+      <c r="F3" s="8">
         <v>6.2</v>
       </c>
-      <c r="H3" s="9">
+      <c r="G3" s="9">
         <v>5.170160240517277E-2</v>
       </c>
-      <c r="I3" s="9"/>
-      <c r="J3" s="10">
+      <c r="H3" s="10">
         <v>125.92</v>
       </c>
-      <c r="K3" s="10"/>
-      <c r="L3" s="8">
-        <v>0</v>
-      </c>
-      <c r="M3" s="8"/>
-      <c r="N3" s="8">
-        <v>0</v>
-      </c>
-      <c r="O3" s="8"/>
-      <c r="P3" s="11">
+      <c r="I3" s="8">
+        <v>0</v>
+      </c>
+      <c r="J3" s="8">
+        <v>0</v>
+      </c>
+      <c r="K3" s="11">
         <v>3.1499999999999972E-2</v>
       </c>
-      <c r="Q3" s="11"/>
-      <c r="R3" s="12">
+      <c r="L3" s="12">
         <v>6.3000000000000003E-4</v>
       </c>
-      <c r="S3" s="13">
+      <c r="M3" s="13">
         <v>5</v>
       </c>
-      <c r="T3" s="13"/>
-      <c r="U3" s="13">
+      <c r="N3" s="13">
         <v>2.3333333333333335</v>
       </c>
-      <c r="V3" s="13"/>
-      <c r="W3" s="13">
+      <c r="O3" s="13">
         <v>2</v>
       </c>
-      <c r="X3" s="13"/>
-      <c r="Y3" s="13">
+      <c r="P3" s="13">
         <v>0.66666666666666663</v>
       </c>
-      <c r="Z3" s="13"/>
-      <c r="AA3" s="13">
+      <c r="Q3" s="13">
         <v>51.499999999999993</v>
       </c>
-      <c r="AB3" s="13"/>
-      <c r="AC3" s="10">
+      <c r="R3" s="10">
         <v>102.33333333333333</v>
       </c>
-      <c r="AD3" s="10"/>
-      <c r="AE3" s="10">
+      <c r="S3" s="10">
         <v>32.777999999999999</v>
       </c>
-      <c r="AF3" s="10">
+      <c r="T3" s="10">
         <v>8.5609999999999999</v>
       </c>
-      <c r="AG3" s="10"/>
-      <c r="AH3" s="10">
-        <v>50</v>
-      </c>
-      <c r="AI3" s="10"/>
-      <c r="AJ3" s="10"/>
-      <c r="AK3" s="8"/>
-    </row>
-    <row r="4" spans="1:37" s="3" customFormat="1">
+    </row>
+    <row r="4" spans="1:20" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A4" s="8">
         <v>2</v>
       </c>
@@ -4235,72 +4134,53 @@
       <c r="E4" s="8">
         <v>0.12</v>
       </c>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8">
+      <c r="F4" s="8">
         <v>6.1</v>
       </c>
-      <c r="H4" s="9">
+      <c r="G4" s="9">
         <v>5.746149602659878E-2</v>
       </c>
-      <c r="I4" s="9"/>
-      <c r="J4" s="10">
+      <c r="H4" s="10">
         <v>124.44333333333334</v>
       </c>
-      <c r="K4" s="10"/>
-      <c r="L4" s="8">
-        <v>0</v>
-      </c>
-      <c r="M4" s="8"/>
-      <c r="N4" s="8">
-        <v>0</v>
-      </c>
-      <c r="O4" s="8"/>
-      <c r="P4" s="11">
+      <c r="I4" s="8">
+        <v>0</v>
+      </c>
+      <c r="J4" s="8">
+        <v>0</v>
+      </c>
+      <c r="K4" s="11">
         <v>7.4999999999999956E-2</v>
       </c>
-      <c r="Q4" s="11"/>
-      <c r="R4" s="12">
+      <c r="L4" s="12">
         <v>1.5299999999999999E-3</v>
       </c>
-      <c r="S4" s="13">
+      <c r="M4" s="13">
         <v>4.333333333333333</v>
       </c>
-      <c r="T4" s="13"/>
-      <c r="U4" s="13">
+      <c r="N4" s="13">
         <v>1</v>
       </c>
-      <c r="V4" s="13"/>
-      <c r="W4" s="13">
+      <c r="O4" s="13">
         <v>3</v>
       </c>
-      <c r="X4" s="13"/>
-      <c r="Y4" s="13">
+      <c r="P4" s="13">
         <v>0.33333333333333331</v>
       </c>
-      <c r="Z4" s="13"/>
-      <c r="AA4" s="13">
+      <c r="Q4" s="13">
         <v>33</v>
       </c>
-      <c r="AB4" s="13"/>
-      <c r="AC4" s="10">
+      <c r="R4" s="10">
         <v>83.5</v>
       </c>
-      <c r="AD4" s="10"/>
-      <c r="AE4" s="10">
+      <c r="S4" s="10">
         <v>32.528000000000006</v>
       </c>
-      <c r="AF4" s="10">
+      <c r="T4" s="10">
         <v>10.274000000000001</v>
       </c>
-      <c r="AG4" s="10"/>
-      <c r="AH4" s="10">
-        <v>50</v>
-      </c>
-      <c r="AI4" s="10"/>
-      <c r="AJ4" s="10"/>
-      <c r="AK4" s="8"/>
-    </row>
-    <row r="5" spans="1:37" s="3" customFormat="1">
+    </row>
+    <row r="5" spans="1:20" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A5" s="8">
         <v>3</v>
       </c>
@@ -4316,72 +4196,53 @@
       <c r="E5" s="8">
         <v>0.11</v>
       </c>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8">
+      <c r="F5" s="8">
         <v>6.25</v>
       </c>
-      <c r="H5" s="9">
+      <c r="G5" s="9">
         <v>6.5721193332475045E-2</v>
       </c>
-      <c r="I5" s="9"/>
-      <c r="J5" s="10">
+      <c r="H5" s="10">
         <v>131.91333333333333</v>
       </c>
-      <c r="K5" s="10"/>
-      <c r="L5" s="8">
+      <c r="I5" s="8">
         <v>2</v>
       </c>
-      <c r="M5" s="8"/>
-      <c r="N5" s="8">
+      <c r="J5" s="8">
         <v>0.32</v>
       </c>
-      <c r="O5" s="8"/>
-      <c r="P5" s="11">
+      <c r="K5" s="11">
         <v>0.1865</v>
       </c>
-      <c r="Q5" s="11"/>
-      <c r="R5" s="12">
+      <c r="L5" s="12">
         <v>6.0299999999999998E-3</v>
       </c>
-      <c r="S5" s="13">
+      <c r="M5" s="13">
         <v>0.33333333333333331</v>
       </c>
-      <c r="T5" s="13"/>
-      <c r="U5" s="13">
+      <c r="N5" s="13">
         <v>0.33333333333333331</v>
       </c>
-      <c r="V5" s="13"/>
-      <c r="W5" s="13">
-        <v>0</v>
-      </c>
-      <c r="X5" s="13"/>
-      <c r="Y5" s="13">
-        <v>0</v>
-      </c>
-      <c r="Z5" s="13"/>
-      <c r="AA5" s="13">
+      <c r="O5" s="13">
+        <v>0</v>
+      </c>
+      <c r="P5" s="13">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="13">
         <v>58.5</v>
       </c>
-      <c r="AB5" s="13"/>
-      <c r="AC5" s="10">
+      <c r="R5" s="10">
         <v>172.33333333333334</v>
       </c>
-      <c r="AD5" s="10"/>
-      <c r="AE5" s="10">
+      <c r="S5" s="10">
         <v>39.453333333333298</v>
       </c>
-      <c r="AF5" s="10">
+      <c r="T5" s="10">
         <v>11.068</v>
       </c>
-      <c r="AG5" s="10"/>
-      <c r="AH5" s="10">
-        <v>50</v>
-      </c>
-      <c r="AI5" s="10"/>
-      <c r="AJ5" s="10"/>
-      <c r="AK5" s="8"/>
-    </row>
-    <row r="6" spans="1:37" s="3" customFormat="1">
+    </row>
+    <row r="6" spans="1:20" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A6" s="8">
         <v>4</v>
       </c>
@@ -4397,72 +4258,53 @@
       <c r="E6" s="8">
         <v>0.12</v>
       </c>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8">
+      <c r="F6" s="8">
         <v>6.2</v>
       </c>
-      <c r="H6" s="9">
+      <c r="G6" s="9">
         <v>4.6389954656435223E-2</v>
       </c>
-      <c r="I6" s="9"/>
-      <c r="J6" s="10">
+      <c r="H6" s="10">
         <v>129.69</v>
       </c>
-      <c r="K6" s="10"/>
-      <c r="L6" s="8">
-        <v>0</v>
-      </c>
-      <c r="M6" s="8"/>
-      <c r="N6" s="8">
-        <v>0</v>
-      </c>
-      <c r="O6" s="8"/>
-      <c r="P6" s="11">
+      <c r="I6" s="8">
+        <v>0</v>
+      </c>
+      <c r="J6" s="8">
+        <v>0</v>
+      </c>
+      <c r="K6" s="11">
         <v>6.0999999999999943E-2</v>
       </c>
-      <c r="Q6" s="11"/>
-      <c r="R6" s="12">
+      <c r="L6" s="12">
         <v>1.89E-3</v>
       </c>
-      <c r="S6" s="13">
-        <v>0</v>
-      </c>
-      <c r="T6" s="13"/>
-      <c r="U6" s="13">
-        <v>0</v>
-      </c>
-      <c r="V6" s="13"/>
-      <c r="W6" s="13">
-        <v>0</v>
-      </c>
-      <c r="X6" s="13"/>
-      <c r="Y6" s="13">
-        <v>0</v>
-      </c>
-      <c r="Z6" s="13"/>
-      <c r="AA6" s="13">
+      <c r="M6" s="13">
+        <v>0</v>
+      </c>
+      <c r="N6" s="13">
+        <v>0</v>
+      </c>
+      <c r="O6" s="13">
+        <v>0</v>
+      </c>
+      <c r="P6" s="13">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="13">
         <v>109</v>
       </c>
-      <c r="AB6" s="13"/>
-      <c r="AC6" s="10">
+      <c r="R6" s="10">
         <v>42.5</v>
       </c>
-      <c r="AD6" s="10"/>
-      <c r="AE6" s="10">
+      <c r="S6" s="10">
         <v>26.339500000000001</v>
       </c>
-      <c r="AF6" s="10">
+      <c r="T6" s="10">
         <v>10.3035</v>
       </c>
-      <c r="AG6" s="10"/>
-      <c r="AH6" s="10">
-        <v>50</v>
-      </c>
-      <c r="AI6" s="10"/>
-      <c r="AJ6" s="10"/>
-      <c r="AK6" s="8"/>
-    </row>
-    <row r="7" spans="1:37" s="3" customFormat="1">
+    </row>
+    <row r="7" spans="1:20" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A7" s="8">
         <v>5</v>
       </c>
@@ -4478,72 +4320,53 @@
       <c r="E7" s="8">
         <v>0.11</v>
       </c>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8">
+      <c r="F7" s="8">
         <v>6.2</v>
       </c>
-      <c r="H7" s="9">
+      <c r="G7" s="9">
         <v>5.1868797026662618E-2</v>
       </c>
-      <c r="I7" s="9"/>
-      <c r="J7" s="10">
+      <c r="H7" s="10">
         <v>125.55500000000001</v>
       </c>
-      <c r="K7" s="10"/>
-      <c r="L7" s="8">
+      <c r="I7" s="8">
         <v>1</v>
       </c>
-      <c r="M7" s="8"/>
-      <c r="N7" s="8">
+      <c r="J7" s="8">
         <v>0.22</v>
       </c>
-      <c r="O7" s="8"/>
-      <c r="P7" s="11">
+      <c r="K7" s="11">
         <v>0.38049999999999995</v>
       </c>
-      <c r="Q7" s="11"/>
-      <c r="R7" s="12">
+      <c r="L7" s="12">
         <v>1.2999999999999999E-2</v>
       </c>
-      <c r="S7" s="13">
+      <c r="M7" s="13">
         <v>9</v>
       </c>
-      <c r="T7" s="13"/>
-      <c r="U7" s="13">
+      <c r="N7" s="13">
         <v>8</v>
       </c>
-      <c r="V7" s="13"/>
-      <c r="W7" s="13">
+      <c r="O7" s="13">
         <v>0.33333333333333331</v>
       </c>
-      <c r="X7" s="13"/>
-      <c r="Y7" s="13">
+      <c r="P7" s="13">
         <v>0.66666666666666663</v>
       </c>
-      <c r="Z7" s="13"/>
-      <c r="AA7" s="13">
+      <c r="Q7" s="13">
         <v>70.666666666666686</v>
       </c>
-      <c r="AB7" s="13"/>
-      <c r="AC7" s="10">
+      <c r="R7" s="10">
         <v>62.666666666666664</v>
       </c>
-      <c r="AD7" s="10"/>
-      <c r="AE7" s="10">
+      <c r="S7" s="10">
         <v>21.807999999999996</v>
       </c>
-      <c r="AF7" s="10">
+      <c r="T7" s="10">
         <v>6.1633333333333331</v>
       </c>
-      <c r="AG7" s="10"/>
-      <c r="AH7" s="10">
-        <v>50</v>
-      </c>
-      <c r="AI7" s="10"/>
-      <c r="AJ7" s="10"/>
-      <c r="AK7" s="8"/>
-    </row>
-    <row r="8" spans="1:37" s="3" customFormat="1">
+    </row>
+    <row r="8" spans="1:20" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A8" s="8">
         <v>6</v>
       </c>
@@ -4559,72 +4382,53 @@
       <c r="E8" s="8">
         <v>0.15</v>
       </c>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8">
+      <c r="F8" s="8">
         <v>4.71</v>
       </c>
-      <c r="H8" s="9">
+      <c r="G8" s="9">
         <v>0.12188071364620238</v>
       </c>
-      <c r="I8" s="9"/>
-      <c r="J8" s="10">
+      <c r="H8" s="10">
         <v>97.1</v>
       </c>
-      <c r="K8" s="10"/>
-      <c r="L8" s="8">
+      <c r="I8" s="8">
         <v>7</v>
       </c>
-      <c r="M8" s="8"/>
-      <c r="N8" s="8">
+      <c r="J8" s="8">
         <v>1.96</v>
       </c>
-      <c r="O8" s="8"/>
-      <c r="P8" s="11">
+      <c r="K8" s="11">
         <v>0.24649999999999994</v>
       </c>
-      <c r="Q8" s="11"/>
-      <c r="R8" s="12">
+      <c r="L8" s="12">
         <v>8.8000000000000005E-3</v>
       </c>
-      <c r="S8" s="13">
+      <c r="M8" s="13">
         <v>66</v>
       </c>
-      <c r="T8" s="13"/>
-      <c r="U8" s="13">
+      <c r="N8" s="13">
         <v>38.333333333333336</v>
       </c>
-      <c r="V8" s="13"/>
-      <c r="W8" s="13">
+      <c r="O8" s="13">
         <v>25.666666666666668</v>
       </c>
-      <c r="X8" s="13"/>
-      <c r="Y8" s="13">
+      <c r="P8" s="13">
         <v>2</v>
       </c>
-      <c r="Z8" s="13"/>
-      <c r="AA8" s="13">
+      <c r="Q8" s="13">
         <v>162.66666666666666</v>
       </c>
-      <c r="AB8" s="13"/>
-      <c r="AC8" s="10">
+      <c r="R8" s="10">
         <v>196.66666666666666</v>
       </c>
-      <c r="AD8" s="10"/>
-      <c r="AE8" s="10">
+      <c r="S8" s="10">
         <v>75.713666666666668</v>
       </c>
-      <c r="AF8" s="10">
+      <c r="T8" s="10">
         <v>10.089333333333334</v>
       </c>
-      <c r="AG8" s="10"/>
-      <c r="AH8" s="10">
-        <v>50</v>
-      </c>
-      <c r="AI8" s="10"/>
-      <c r="AJ8" s="10"/>
-      <c r="AK8" s="8"/>
-    </row>
-    <row r="9" spans="1:37" s="3" customFormat="1">
+    </row>
+    <row r="9" spans="1:20" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A9" s="8">
         <v>7</v>
       </c>
@@ -4640,72 +4444,53 @@
       <c r="E9" s="8">
         <v>0.16</v>
       </c>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8">
+      <c r="F9" s="8">
         <v>5.51</v>
       </c>
-      <c r="H9" s="9">
+      <c r="G9" s="9">
         <v>0.10836036120643874</v>
       </c>
-      <c r="I9" s="9"/>
-      <c r="J9" s="10">
+      <c r="H9" s="10">
         <v>122.68666666666667</v>
       </c>
-      <c r="K9" s="10"/>
-      <c r="L9" s="8">
+      <c r="I9" s="8">
         <v>13</v>
       </c>
-      <c r="M9" s="8"/>
-      <c r="N9" s="8">
+      <c r="J9" s="8">
         <v>1.74</v>
       </c>
-      <c r="O9" s="8"/>
-      <c r="P9" s="11">
+      <c r="K9" s="11">
         <v>0.14600000000000013</v>
       </c>
-      <c r="Q9" s="11"/>
-      <c r="R9" s="12">
+      <c r="L9" s="12">
         <v>5.3400000000000001E-3</v>
       </c>
-      <c r="S9" s="13">
+      <c r="M9" s="13">
         <v>29</v>
       </c>
-      <c r="T9" s="13"/>
-      <c r="U9" s="13">
+      <c r="N9" s="13">
         <v>18</v>
       </c>
-      <c r="V9" s="13"/>
-      <c r="W9" s="13">
+      <c r="O9" s="13">
         <v>9.3333333333333339</v>
       </c>
-      <c r="X9" s="13"/>
-      <c r="Y9" s="13">
+      <c r="P9" s="13">
         <v>1.6666666666666667</v>
       </c>
-      <c r="Z9" s="13"/>
-      <c r="AA9" s="13">
+      <c r="Q9" s="13">
         <v>153.75</v>
       </c>
-      <c r="AB9" s="13"/>
-      <c r="AC9" s="10">
+      <c r="R9" s="10">
         <v>220.25</v>
       </c>
-      <c r="AD9" s="10"/>
-      <c r="AE9" s="10">
+      <c r="S9" s="10">
         <v>59.065750000000001</v>
       </c>
-      <c r="AF9" s="10">
+      <c r="T9" s="10">
         <v>12.58825</v>
       </c>
-      <c r="AG9" s="10"/>
-      <c r="AH9" s="10">
-        <v>50</v>
-      </c>
-      <c r="AI9" s="10"/>
-      <c r="AJ9" s="10"/>
-      <c r="AK9" s="8"/>
-    </row>
-    <row r="10" spans="1:37" s="3" customFormat="1">
+    </row>
+    <row r="10" spans="1:20" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A10" s="8">
         <v>8</v>
       </c>
@@ -4721,72 +4506,53 @@
       <c r="E10" s="8">
         <v>0.13</v>
       </c>
-      <c r="F10" s="8"/>
-      <c r="G10" s="8">
+      <c r="F10" s="8">
         <v>5.38</v>
       </c>
-      <c r="H10" s="9">
+      <c r="G10" s="9">
         <v>0.11629427746722501</v>
       </c>
-      <c r="I10" s="9"/>
-      <c r="J10" s="10">
+      <c r="H10" s="10">
         <v>120.63666666666666</v>
       </c>
-      <c r="K10" s="10"/>
-      <c r="L10" s="8">
+      <c r="I10" s="8">
         <v>6</v>
       </c>
-      <c r="M10" s="8"/>
-      <c r="N10" s="8">
+      <c r="J10" s="8">
         <v>2.94</v>
       </c>
-      <c r="O10" s="8"/>
-      <c r="P10" s="11">
+      <c r="K10" s="11">
         <v>0.29849999999999999</v>
       </c>
-      <c r="Q10" s="11"/>
-      <c r="R10" s="12">
+      <c r="L10" s="12">
         <v>9.4500000000000001E-3</v>
       </c>
-      <c r="S10" s="13">
+      <c r="M10" s="13">
         <v>68</v>
       </c>
-      <c r="T10" s="13"/>
-      <c r="U10" s="13">
+      <c r="N10" s="13">
         <v>10</v>
       </c>
-      <c r="V10" s="13"/>
-      <c r="W10" s="13">
+      <c r="O10" s="13">
         <v>54</v>
       </c>
-      <c r="X10" s="13"/>
-      <c r="Y10" s="13">
+      <c r="P10" s="13">
         <v>4</v>
       </c>
-      <c r="Z10" s="13"/>
-      <c r="AA10" s="13">
+      <c r="Q10" s="13">
         <v>133.5</v>
       </c>
-      <c r="AB10" s="13"/>
-      <c r="AC10" s="10">
+      <c r="R10" s="10">
         <v>112</v>
       </c>
-      <c r="AD10" s="10"/>
-      <c r="AE10" s="10">
+      <c r="S10" s="10">
         <v>48.877499999999998</v>
       </c>
-      <c r="AF10" s="10">
+      <c r="T10" s="10">
         <v>12.092500000000001</v>
       </c>
-      <c r="AG10" s="10"/>
-      <c r="AH10" s="10">
-        <v>50</v>
-      </c>
-      <c r="AI10" s="10"/>
-      <c r="AJ10" s="10"/>
-      <c r="AK10" s="8"/>
-    </row>
-    <row r="11" spans="1:37" s="3" customFormat="1">
+    </row>
+    <row r="11" spans="1:20" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A11" s="8">
         <v>9</v>
       </c>
@@ -4802,72 +4568,53 @@
       <c r="E11" s="8">
         <v>0.17</v>
       </c>
-      <c r="F11" s="8"/>
-      <c r="G11" s="8">
+      <c r="F11" s="8">
         <v>4.71</v>
       </c>
-      <c r="H11" s="9">
+      <c r="G11" s="9">
         <v>0.15633440325674258</v>
       </c>
-      <c r="I11" s="9"/>
-      <c r="J11" s="10">
+      <c r="H11" s="10">
         <v>119.43333333333334</v>
       </c>
-      <c r="K11" s="10"/>
-      <c r="L11" s="8">
+      <c r="I11" s="8">
         <v>10</v>
       </c>
-      <c r="M11" s="8"/>
-      <c r="N11" s="8">
+      <c r="J11" s="8">
         <v>3.02</v>
       </c>
-      <c r="O11" s="8"/>
-      <c r="P11" s="11">
+      <c r="K11" s="11">
         <v>9.000000000000008E-2</v>
       </c>
-      <c r="Q11" s="11"/>
-      <c r="R11" s="12">
+      <c r="L11" s="12">
         <v>3.3700000000000002E-3</v>
       </c>
-      <c r="S11" s="13">
+      <c r="M11" s="13">
         <v>42</v>
       </c>
-      <c r="T11" s="13"/>
-      <c r="U11" s="13">
+      <c r="N11" s="13">
         <v>20.333333333333332</v>
       </c>
-      <c r="V11" s="13"/>
-      <c r="W11" s="13">
+      <c r="O11" s="13">
         <v>20</v>
       </c>
-      <c r="X11" s="13"/>
-      <c r="Y11" s="13">
+      <c r="P11" s="13">
         <v>1.6666666666666667</v>
       </c>
-      <c r="Z11" s="13"/>
-      <c r="AA11" s="13">
+      <c r="Q11" s="13">
         <v>181</v>
       </c>
-      <c r="AB11" s="13"/>
-      <c r="AC11" s="10">
+      <c r="R11" s="10">
         <v>147.5</v>
       </c>
-      <c r="AD11" s="10"/>
-      <c r="AE11" s="10">
+      <c r="S11" s="10">
         <v>65.393000000000001</v>
       </c>
-      <c r="AF11" s="10">
+      <c r="T11" s="10">
         <v>18.207000000000001</v>
       </c>
-      <c r="AG11" s="10"/>
-      <c r="AH11" s="10">
-        <v>50</v>
-      </c>
-      <c r="AI11" s="10"/>
-      <c r="AJ11" s="10"/>
-      <c r="AK11" s="8"/>
-    </row>
-    <row r="12" spans="1:37" s="3" customFormat="1">
+    </row>
+    <row r="12" spans="1:20" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A12" s="8">
         <v>10</v>
       </c>
@@ -4883,72 +4630,53 @@
       <c r="E12" s="8">
         <v>0.16</v>
       </c>
-      <c r="F12" s="8"/>
-      <c r="G12" s="8">
+      <c r="F12" s="8">
         <v>4.7300000000000004</v>
       </c>
-      <c r="H12" s="9">
+      <c r="G12" s="9">
         <v>0.13149379914290241</v>
       </c>
-      <c r="I12" s="9"/>
-      <c r="J12" s="10">
+      <c r="H12" s="10">
         <v>127.46666666666665</v>
       </c>
-      <c r="K12" s="10"/>
-      <c r="L12" s="8">
+      <c r="I12" s="8">
         <v>12</v>
       </c>
-      <c r="M12" s="8"/>
-      <c r="N12" s="8">
+      <c r="J12" s="8">
         <v>5.82</v>
       </c>
-      <c r="O12" s="8"/>
-      <c r="P12" s="11">
+      <c r="K12" s="11">
         <v>0.18450000000000011</v>
       </c>
-      <c r="Q12" s="11"/>
-      <c r="R12" s="12">
+      <c r="L12" s="12">
         <v>3.7499999999999999E-3</v>
       </c>
-      <c r="S12" s="13">
+      <c r="M12" s="13">
         <v>51.333333333333336</v>
       </c>
-      <c r="T12" s="13"/>
-      <c r="U12" s="13">
+      <c r="N12" s="13">
         <v>12.333333333333334</v>
       </c>
-      <c r="V12" s="13"/>
-      <c r="W12" s="13">
+      <c r="O12" s="13">
         <v>37.666666666666664</v>
       </c>
-      <c r="X12" s="13"/>
-      <c r="Y12" s="13">
+      <c r="P12" s="13">
         <v>1.3333333333333333</v>
       </c>
-      <c r="Z12" s="13"/>
-      <c r="AA12" s="13">
+      <c r="Q12" s="13">
         <v>163.33333333333337</v>
       </c>
-      <c r="AB12" s="13"/>
-      <c r="AC12" s="10">
+      <c r="R12" s="10">
         <v>336.66666666666669</v>
       </c>
-      <c r="AD12" s="10"/>
-      <c r="AE12" s="10">
+      <c r="S12" s="10">
         <v>53.199666666666666</v>
       </c>
-      <c r="AF12" s="10">
+      <c r="T12" s="10">
         <v>15.343999999999999</v>
       </c>
-      <c r="AG12" s="10"/>
-      <c r="AH12" s="10">
-        <v>50</v>
-      </c>
-      <c r="AI12" s="10"/>
-      <c r="AJ12" s="10"/>
-      <c r="AK12" s="8"/>
-    </row>
-    <row r="13" spans="1:37" s="3" customFormat="1">
+    </row>
+    <row r="13" spans="1:20" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
         <v>11</v>
       </c>
@@ -4964,68 +4692,53 @@
       <c r="E13" s="3">
         <v>0.27</v>
       </c>
-      <c r="G13" s="3">
+      <c r="F13" s="3">
         <v>3.55</v>
       </c>
-      <c r="H13" s="14">
+      <c r="G13" s="14">
         <v>0.15306201887328777</v>
       </c>
-      <c r="I13" s="14"/>
-      <c r="J13" s="15">
+      <c r="H13" s="15">
         <v>91.83</v>
       </c>
-      <c r="K13" s="15"/>
-      <c r="L13" s="3">
+      <c r="I13" s="3">
         <v>13</v>
       </c>
-      <c r="N13" s="3">
+      <c r="J13" s="3">
         <v>1.54</v>
       </c>
-      <c r="P13" s="16">
+      <c r="K13" s="16">
         <v>4.9499999999999877E-2</v>
       </c>
-      <c r="Q13" s="16"/>
-      <c r="R13" s="17">
+      <c r="L13" s="17">
         <v>4.3800000000000002E-3</v>
       </c>
-      <c r="S13" s="18">
+      <c r="M13" s="18">
         <v>67.666666666666671</v>
       </c>
-      <c r="T13" s="18"/>
-      <c r="U13" s="18">
+      <c r="N13" s="18">
         <v>22</v>
       </c>
-      <c r="V13" s="18"/>
-      <c r="W13" s="18">
+      <c r="O13" s="18">
         <v>40.333333333333336</v>
       </c>
-      <c r="X13" s="18"/>
-      <c r="Y13" s="18">
+      <c r="P13" s="18">
         <v>5.333333333333333</v>
       </c>
-      <c r="Z13" s="18"/>
-      <c r="AA13" s="18">
+      <c r="Q13" s="18">
         <v>169.20000000000002</v>
       </c>
-      <c r="AB13" s="18"/>
-      <c r="AC13" s="15">
+      <c r="R13" s="15">
         <v>182.2</v>
       </c>
-      <c r="AD13" s="15"/>
-      <c r="AE13" s="15">
+      <c r="S13" s="15">
         <v>100.422</v>
       </c>
-      <c r="AF13" s="15">
+      <c r="T13" s="15">
         <v>18.593800000000002</v>
       </c>
-      <c r="AG13" s="15"/>
-      <c r="AH13" s="10">
-        <v>50</v>
-      </c>
-      <c r="AI13" s="15"/>
-      <c r="AJ13" s="15"/>
-    </row>
-    <row r="14" spans="1:37" s="3" customFormat="1">
+    </row>
+    <row r="14" spans="1:20" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A14" s="8">
         <v>12</v>
       </c>
@@ -5041,72 +4754,53 @@
       <c r="E14" s="8">
         <v>0.26</v>
       </c>
-      <c r="F14" s="8"/>
-      <c r="G14" s="8">
+      <c r="F14" s="8">
         <v>3.54</v>
       </c>
-      <c r="H14" s="9">
+      <c r="G14" s="9">
         <v>0.15680760687121015</v>
       </c>
-      <c r="I14" s="9"/>
-      <c r="J14" s="10">
+      <c r="H14" s="10">
         <v>81.913333333333341</v>
       </c>
-      <c r="K14" s="10"/>
-      <c r="L14" s="8">
+      <c r="I14" s="8">
         <v>4</v>
       </c>
-      <c r="M14" s="8"/>
-      <c r="N14" s="8">
+      <c r="J14" s="8">
         <v>1.0900000000000001</v>
       </c>
-      <c r="O14" s="8"/>
-      <c r="P14" s="11">
+      <c r="K14" s="11">
         <v>0.14649999999999996</v>
       </c>
-      <c r="Q14" s="11"/>
-      <c r="R14" s="12">
+      <c r="L14" s="12">
         <v>3.32E-3</v>
       </c>
-      <c r="S14" s="13">
+      <c r="M14" s="13">
         <v>122.33333333333333</v>
       </c>
-      <c r="T14" s="13"/>
-      <c r="U14" s="13">
+      <c r="N14" s="13">
         <v>81.666666666666671</v>
       </c>
-      <c r="V14" s="13"/>
-      <c r="W14" s="13">
+      <c r="O14" s="13">
         <v>33</v>
       </c>
-      <c r="X14" s="13"/>
-      <c r="Y14" s="13">
+      <c r="P14" s="13">
         <v>7.666666666666667</v>
       </c>
-      <c r="Z14" s="13"/>
-      <c r="AA14" s="13">
+      <c r="Q14" s="13">
         <v>170.5</v>
       </c>
-      <c r="AB14" s="13"/>
-      <c r="AC14" s="10">
+      <c r="R14" s="10">
         <v>27</v>
       </c>
-      <c r="AD14" s="10"/>
-      <c r="AE14" s="10">
+      <c r="S14" s="10">
         <v>72.88033333333334</v>
       </c>
-      <c r="AF14" s="10">
+      <c r="T14" s="10">
         <v>18.944666666666667</v>
       </c>
-      <c r="AG14" s="10"/>
-      <c r="AH14" s="10">
-        <v>50</v>
-      </c>
-      <c r="AI14" s="10"/>
-      <c r="AJ14" s="10"/>
-      <c r="AK14" s="8"/>
-    </row>
-    <row r="15" spans="1:37" s="3" customFormat="1">
+    </row>
+    <row r="15" spans="1:20" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A15" s="8">
         <v>13</v>
       </c>
@@ -5122,72 +4816,53 @@
       <c r="E15" s="8">
         <v>0.33</v>
       </c>
-      <c r="F15" s="8"/>
-      <c r="G15" s="8">
+      <c r="F15" s="8">
         <v>3.51</v>
       </c>
-      <c r="H15" s="9">
+      <c r="G15" s="9">
         <v>0.23684373097214709</v>
       </c>
-      <c r="I15" s="9"/>
-      <c r="J15" s="10">
+      <c r="H15" s="10">
         <v>85.663333333333341</v>
       </c>
-      <c r="K15" s="10"/>
-      <c r="L15" s="8">
+      <c r="I15" s="8">
         <v>9</v>
       </c>
-      <c r="M15" s="8"/>
-      <c r="N15" s="8">
+      <c r="J15" s="8">
         <v>0.97</v>
       </c>
-      <c r="O15" s="8"/>
-      <c r="P15" s="11">
+      <c r="K15" s="11">
         <v>4.3999999999999928E-2</v>
       </c>
-      <c r="Q15" s="11"/>
-      <c r="R15" s="12">
+      <c r="L15" s="12">
         <v>1.23E-3</v>
       </c>
-      <c r="S15" s="13">
+      <c r="M15" s="13">
         <v>115.5</v>
       </c>
-      <c r="T15" s="13"/>
-      <c r="U15" s="13">
+      <c r="N15" s="13">
         <v>84</v>
       </c>
-      <c r="V15" s="13"/>
-      <c r="W15" s="13">
+      <c r="O15" s="13">
         <v>13.5</v>
       </c>
-      <c r="X15" s="13"/>
-      <c r="Y15" s="13">
+      <c r="P15" s="13">
         <v>18</v>
       </c>
-      <c r="Z15" s="13"/>
-      <c r="AA15" s="13">
+      <c r="Q15" s="13">
         <v>231.5</v>
       </c>
-      <c r="AB15" s="13"/>
-      <c r="AC15" s="10">
+      <c r="R15" s="10">
         <v>140</v>
       </c>
-      <c r="AD15" s="10"/>
-      <c r="AE15" s="10">
+      <c r="S15" s="10">
         <v>110.742</v>
       </c>
-      <c r="AF15" s="10">
+      <c r="T15" s="10">
         <v>25.585000000000001</v>
       </c>
-      <c r="AG15" s="10"/>
-      <c r="AH15" s="10">
-        <v>50</v>
-      </c>
-      <c r="AI15" s="10"/>
-      <c r="AJ15" s="10"/>
-      <c r="AK15" s="8"/>
-    </row>
-    <row r="16" spans="1:37" s="3" customFormat="1">
+    </row>
+    <row r="16" spans="1:20" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A16" s="8">
         <v>14</v>
       </c>
@@ -5203,72 +4878,53 @@
       <c r="E16" s="8">
         <v>0.32</v>
       </c>
-      <c r="F16" s="8"/>
-      <c r="G16" s="8">
+      <c r="F16" s="8">
         <v>3.47</v>
       </c>
-      <c r="H16" s="9">
+      <c r="G16" s="9">
         <v>0.20300924642106569</v>
       </c>
-      <c r="I16" s="9"/>
-      <c r="J16" s="10">
+      <c r="H16" s="10">
         <v>95.570000000000007</v>
       </c>
-      <c r="K16" s="10"/>
-      <c r="L16" s="8">
-        <v>0</v>
-      </c>
-      <c r="M16" s="8"/>
-      <c r="N16" s="8">
-        <v>0</v>
-      </c>
-      <c r="O16" s="8"/>
-      <c r="P16" s="11">
+      <c r="I16" s="8">
+        <v>0</v>
+      </c>
+      <c r="J16" s="8">
+        <v>0</v>
+      </c>
+      <c r="K16" s="11">
         <v>4.049999999999998E-2</v>
       </c>
-      <c r="Q16" s="11"/>
-      <c r="R16" s="12">
+      <c r="L16" s="12">
         <v>3.7699999999999999E-3</v>
       </c>
-      <c r="S16" s="13">
+      <c r="M16" s="13">
         <v>34</v>
       </c>
-      <c r="T16" s="13"/>
-      <c r="U16" s="13">
+      <c r="N16" s="13">
         <v>7.5</v>
       </c>
-      <c r="V16" s="13"/>
-      <c r="W16" s="13">
+      <c r="O16" s="13">
         <v>5</v>
       </c>
-      <c r="X16" s="13"/>
-      <c r="Y16" s="13">
+      <c r="P16" s="13">
         <v>4</v>
       </c>
-      <c r="Z16" s="13"/>
-      <c r="AA16" s="13">
+      <c r="Q16" s="13">
         <v>222.33333333333334</v>
       </c>
-      <c r="AB16" s="13"/>
-      <c r="AC16" s="10">
+      <c r="R16" s="10">
         <v>31.333333333333332</v>
       </c>
-      <c r="AD16" s="10"/>
-      <c r="AE16" s="10">
+      <c r="S16" s="10">
         <v>100.29833333333333</v>
       </c>
-      <c r="AF16" s="10">
+      <c r="T16" s="10">
         <v>34.152000000000001</v>
       </c>
-      <c r="AG16" s="10"/>
-      <c r="AH16" s="10">
-        <v>50</v>
-      </c>
-      <c r="AI16" s="10"/>
-      <c r="AJ16" s="10"/>
-      <c r="AK16" s="8"/>
-    </row>
-    <row r="17" spans="1:37" s="3" customFormat="1">
+    </row>
+    <row r="17" spans="1:20" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A17" s="8">
         <v>15</v>
       </c>
@@ -5284,72 +4940,53 @@
       <c r="E17" s="8">
         <v>0.25</v>
       </c>
-      <c r="F17" s="8"/>
-      <c r="G17" s="8">
+      <c r="F17" s="8">
         <v>3.5</v>
       </c>
-      <c r="H17" s="9">
+      <c r="G17" s="9">
         <v>0.22380437855993457</v>
       </c>
-      <c r="I17" s="9"/>
-      <c r="J17" s="10">
+      <c r="H17" s="10">
         <v>70.775000000000006</v>
       </c>
-      <c r="K17" s="10"/>
-      <c r="L17" s="8">
+      <c r="I17" s="8">
         <v>6</v>
       </c>
-      <c r="M17" s="8"/>
-      <c r="N17" s="8">
+      <c r="J17" s="8">
         <v>0.65</v>
       </c>
-      <c r="O17" s="8"/>
-      <c r="P17" s="11">
+      <c r="K17" s="11">
         <v>0.21199999999999997</v>
       </c>
-      <c r="Q17" s="11"/>
-      <c r="R17" s="12">
+      <c r="L17" s="12">
         <v>8.8199999999999997E-3</v>
       </c>
-      <c r="S17" s="13">
+      <c r="M17" s="13">
         <v>55.5</v>
       </c>
-      <c r="T17" s="13"/>
-      <c r="U17" s="13">
+      <c r="N17" s="13">
         <v>40.5</v>
       </c>
-      <c r="V17" s="13"/>
-      <c r="W17" s="13">
+      <c r="O17" s="13">
         <v>5.5</v>
       </c>
-      <c r="X17" s="13"/>
-      <c r="Y17" s="13">
+      <c r="P17" s="13">
         <v>9</v>
       </c>
-      <c r="Z17" s="13"/>
-      <c r="AA17" s="13">
+      <c r="Q17" s="13">
         <v>130.00000000000003</v>
       </c>
-      <c r="AB17" s="13"/>
-      <c r="AC17" s="10">
+      <c r="R17" s="10">
         <v>119</v>
       </c>
-      <c r="AD17" s="10"/>
-      <c r="AE17" s="10">
+      <c r="S17" s="10">
         <v>100.23400000000001</v>
       </c>
-      <c r="AF17" s="10">
+      <c r="T17" s="10">
         <v>14.298999999999999</v>
       </c>
-      <c r="AG17" s="10"/>
-      <c r="AH17" s="10">
-        <v>50</v>
-      </c>
-      <c r="AI17" s="10"/>
-      <c r="AJ17" s="10"/>
-      <c r="AK17" s="8"/>
-    </row>
-    <row r="18" spans="1:37" s="3" customFormat="1">
+    </row>
+    <row r="18" spans="1:20" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A18" s="3">
         <v>16</v>
       </c>
@@ -5365,59 +5002,44 @@
       <c r="E18" s="3">
         <v>0.17</v>
       </c>
-      <c r="H18" s="14">
+      <c r="G18" s="14">
         <v>0.22456461961503188</v>
       </c>
-      <c r="I18" s="14"/>
-      <c r="K18" s="15"/>
-      <c r="L18" s="3">
+      <c r="I18" s="3">
         <v>56</v>
       </c>
+      <c r="J18" s="3">
+        <v>10.6</v>
+      </c>
+      <c r="L18" s="17">
+        <v>9.11E-3</v>
+      </c>
+      <c r="M18" s="3">
+        <v>8</v>
+      </c>
       <c r="N18" s="3">
-        <v>10.6</v>
-      </c>
-      <c r="Q18" s="16"/>
-      <c r="R18" s="17">
-        <v>9.11E-3</v>
-      </c>
-      <c r="S18" s="3">
-        <v>8</v>
-      </c>
-      <c r="T18" s="18"/>
-      <c r="U18" s="3">
         <v>3</v>
       </c>
-      <c r="V18" s="18"/>
-      <c r="W18" s="3">
+      <c r="O18" s="3">
         <v>5</v>
       </c>
-      <c r="X18" s="18"/>
-      <c r="Y18" s="3">
-        <v>0</v>
-      </c>
-      <c r="Z18" s="18"/>
-      <c r="AA18" s="18">
+      <c r="P18" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q18" s="18">
         <v>169.23556565999999</v>
       </c>
-      <c r="AB18" s="18"/>
-      <c r="AC18" s="3">
+      <c r="R18" s="3">
         <v>84</v>
       </c>
-      <c r="AD18" s="15"/>
-      <c r="AE18" s="15">
+      <c r="S18" s="15">
         <v>65.224000000000004</v>
       </c>
-      <c r="AF18" s="15">
+      <c r="T18" s="15">
         <v>13.547000000000001</v>
       </c>
-      <c r="AG18" s="15"/>
-      <c r="AH18" s="10">
-        <v>50</v>
-      </c>
-      <c r="AI18" s="15"/>
-      <c r="AJ18" s="15"/>
-    </row>
-    <row r="19" spans="1:37" s="3" customFormat="1">
+    </row>
+    <row r="19" spans="1:20" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A19" s="3">
         <v>17</v>
       </c>
@@ -5433,59 +5055,44 @@
       <c r="E19" s="3">
         <v>0.21000000000000002</v>
       </c>
-      <c r="H19" s="14">
+      <c r="G19" s="14">
         <v>0.15926157697121415</v>
       </c>
-      <c r="I19" s="14"/>
-      <c r="K19" s="15"/>
-      <c r="L19" s="3">
+      <c r="I19" s="3">
         <v>54</v>
       </c>
+      <c r="J19" s="3">
+        <v>6.78</v>
+      </c>
+      <c r="L19" s="17">
+        <v>8.8749999999999992E-3</v>
+      </c>
+      <c r="M19" s="3">
+        <v>27</v>
+      </c>
       <c r="N19" s="3">
-        <v>6.78</v>
-      </c>
-      <c r="Q19" s="16"/>
-      <c r="R19" s="17">
-        <v>8.8749999999999992E-3</v>
-      </c>
-      <c r="S19" s="3">
-        <v>27</v>
-      </c>
-      <c r="T19" s="18"/>
-      <c r="U19" s="3">
         <v>14</v>
       </c>
-      <c r="V19" s="18"/>
-      <c r="W19" s="3">
+      <c r="O19" s="3">
         <v>11</v>
       </c>
-      <c r="X19" s="18"/>
-      <c r="Y19" s="3">
+      <c r="P19" s="3">
         <v>2</v>
       </c>
-      <c r="Z19" s="18"/>
-      <c r="AA19" s="18">
+      <c r="Q19" s="18">
         <v>120.30811786500001</v>
       </c>
-      <c r="AB19" s="18"/>
-      <c r="AC19" s="3">
+      <c r="R19" s="3">
         <v>174</v>
       </c>
-      <c r="AD19" s="15"/>
-      <c r="AE19" s="15">
+      <c r="S19" s="15">
         <v>82.552000000000007</v>
       </c>
-      <c r="AF19" s="15">
+      <c r="T19" s="15">
         <v>16.373999999999999</v>
       </c>
-      <c r="AG19" s="15"/>
-      <c r="AH19" s="10">
-        <v>50</v>
-      </c>
-      <c r="AI19" s="15"/>
-      <c r="AJ19" s="15"/>
-    </row>
-    <row r="20" spans="1:37" s="3" customFormat="1">
+    </row>
+    <row r="20" spans="1:20" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A20" s="3">
         <v>18</v>
       </c>
@@ -5501,59 +5108,44 @@
       <c r="E20" s="3">
         <v>0.14000000000000001</v>
       </c>
-      <c r="H20" s="14">
+      <c r="G20" s="14">
         <v>0.13666870042708984</v>
       </c>
-      <c r="I20" s="14"/>
-      <c r="K20" s="15"/>
-      <c r="L20" s="3">
+      <c r="I20" s="3">
         <v>14</v>
       </c>
+      <c r="J20" s="3">
+        <v>3.18</v>
+      </c>
+      <c r="L20" s="17">
+        <v>1.7510000000000001E-2</v>
+      </c>
+      <c r="M20" s="3">
+        <v>1</v>
+      </c>
       <c r="N20" s="3">
-        <v>3.18</v>
-      </c>
-      <c r="Q20" s="16"/>
-      <c r="R20" s="17">
-        <v>1.7510000000000001E-2</v>
-      </c>
-      <c r="S20" s="3">
         <v>1</v>
       </c>
-      <c r="T20" s="18"/>
-      <c r="U20" s="3">
-        <v>1</v>
-      </c>
-      <c r="V20" s="18"/>
-      <c r="W20" s="3">
-        <v>0</v>
-      </c>
-      <c r="X20" s="18"/>
-      <c r="Y20" s="3">
-        <v>0</v>
-      </c>
-      <c r="Z20" s="18"/>
-      <c r="AA20" s="18">
+      <c r="O20" s="3">
+        <v>0</v>
+      </c>
+      <c r="P20" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q20" s="18">
         <v>60.190075625999988</v>
       </c>
-      <c r="AB20" s="18"/>
-      <c r="AC20" s="3">
+      <c r="R20" s="3">
         <v>272</v>
       </c>
-      <c r="AD20" s="15"/>
-      <c r="AE20" s="15">
+      <c r="S20" s="15">
         <v>55.939</v>
       </c>
-      <c r="AF20" s="15">
+      <c r="T20" s="15">
         <v>6.7069999999999999</v>
       </c>
-      <c r="AG20" s="15"/>
-      <c r="AH20" s="10">
-        <v>50</v>
-      </c>
-      <c r="AI20" s="15"/>
-      <c r="AJ20" s="15"/>
-    </row>
-    <row r="21" spans="1:37" s="3" customFormat="1">
+    </row>
+    <row r="21" spans="1:20" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A21" s="3">
         <v>19</v>
       </c>
@@ -5569,59 +5161,44 @@
       <c r="E21" s="3">
         <v>0.16</v>
       </c>
-      <c r="H21" s="14">
+      <c r="G21" s="14">
         <v>0.22867110688233452</v>
       </c>
-      <c r="I21" s="14"/>
-      <c r="K21" s="15"/>
-      <c r="L21" s="3">
+      <c r="I21" s="3">
         <v>44</v>
       </c>
+      <c r="J21" s="3">
+        <v>8.76</v>
+      </c>
+      <c r="L21" s="17">
+        <v>6.659E-3</v>
+      </c>
+      <c r="M21" s="3">
+        <v>43</v>
+      </c>
       <c r="N21" s="3">
-        <v>8.76</v>
-      </c>
-      <c r="Q21" s="16"/>
-      <c r="R21" s="17">
-        <v>6.659E-3</v>
-      </c>
-      <c r="S21" s="3">
-        <v>43</v>
-      </c>
-      <c r="T21" s="18"/>
-      <c r="U21" s="3">
         <v>40</v>
       </c>
-      <c r="V21" s="18"/>
-      <c r="W21" s="3">
+      <c r="O21" s="3">
         <v>3</v>
       </c>
-      <c r="X21" s="18"/>
-      <c r="Y21" s="3">
-        <v>0</v>
-      </c>
-      <c r="Z21" s="18"/>
-      <c r="AA21" s="18">
+      <c r="P21" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q21" s="18">
         <v>145.35676359000001</v>
       </c>
-      <c r="AB21" s="18"/>
-      <c r="AC21" s="3">
+      <c r="R21" s="3">
         <v>153</v>
       </c>
-      <c r="AD21" s="15"/>
-      <c r="AE21" s="15">
+      <c r="S21" s="15">
         <v>81.656000000000006</v>
       </c>
-      <c r="AF21" s="15">
+      <c r="T21" s="15">
         <v>16.376999999999999</v>
       </c>
-      <c r="AG21" s="15"/>
-      <c r="AH21" s="10">
-        <v>50</v>
-      </c>
-      <c r="AI21" s="15"/>
-      <c r="AJ21" s="15"/>
-    </row>
-    <row r="22" spans="1:37" s="3" customFormat="1">
+    </row>
+    <row r="22" spans="1:20" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A22" s="3">
         <v>20</v>
       </c>
@@ -5637,59 +5214,44 @@
       <c r="E22" s="3">
         <v>0.2</v>
       </c>
-      <c r="H22" s="14">
+      <c r="G22" s="14">
         <v>0.28716216216216228</v>
       </c>
-      <c r="I22" s="14"/>
-      <c r="K22" s="15"/>
-      <c r="L22" s="3">
+      <c r="I22" s="3">
         <v>4</v>
       </c>
+      <c r="J22" s="3">
+        <v>0.18</v>
+      </c>
+      <c r="L22" s="17">
+        <v>1.2290000000000001E-2</v>
+      </c>
+      <c r="M22" s="3">
+        <v>6</v>
+      </c>
       <c r="N22" s="3">
-        <v>0.18</v>
-      </c>
-      <c r="Q22" s="16"/>
-      <c r="R22" s="17">
-        <v>1.2290000000000001E-2</v>
-      </c>
-      <c r="S22" s="3">
-        <v>6</v>
-      </c>
-      <c r="T22" s="18"/>
-      <c r="U22" s="3">
         <v>4</v>
       </c>
-      <c r="V22" s="18"/>
-      <c r="W22" s="3">
+      <c r="O22" s="3">
         <v>1</v>
       </c>
-      <c r="X22" s="18"/>
-      <c r="Y22" s="3">
+      <c r="P22" s="3">
         <v>1</v>
       </c>
-      <c r="Z22" s="18"/>
-      <c r="AA22" s="18">
+      <c r="Q22" s="18">
         <v>65.536068674999996</v>
       </c>
-      <c r="AB22" s="18"/>
-      <c r="AC22" s="3">
+      <c r="R22" s="3">
         <v>35</v>
       </c>
-      <c r="AD22" s="15"/>
-      <c r="AE22" s="15">
+      <c r="S22" s="15">
         <v>66.64200000000001</v>
       </c>
-      <c r="AF22" s="15">
+      <c r="T22" s="15">
         <v>16.660999999999998</v>
       </c>
-      <c r="AG22" s="15"/>
-      <c r="AH22" s="10">
-        <v>50</v>
-      </c>
-      <c r="AI22" s="15"/>
-      <c r="AJ22" s="15"/>
-    </row>
-    <row r="23" spans="1:37" s="3" customFormat="1">
+    </row>
+    <row r="23" spans="1:20" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A23" s="3">
         <v>21</v>
       </c>
@@ -5705,59 +5267,44 @@
       <c r="E23" s="3">
         <v>0.3</v>
       </c>
-      <c r="H23" s="14">
+      <c r="G23" s="14">
         <v>0.25470514429109176</v>
       </c>
-      <c r="I23" s="14"/>
-      <c r="K23" s="15"/>
-      <c r="L23" s="3">
+      <c r="I23" s="3">
         <v>6</v>
       </c>
+      <c r="J23" s="3">
+        <v>2.76</v>
+      </c>
+      <c r="L23" s="17">
+        <v>9.8989999999999998E-3</v>
+      </c>
+      <c r="M23" s="3">
+        <v>18</v>
+      </c>
       <c r="N23" s="3">
-        <v>2.76</v>
-      </c>
-      <c r="Q23" s="16"/>
-      <c r="R23" s="17">
-        <v>9.8989999999999998E-3</v>
-      </c>
-      <c r="S23" s="3">
-        <v>18</v>
-      </c>
-      <c r="T23" s="18"/>
-      <c r="U23" s="3">
-        <v>0</v>
-      </c>
-      <c r="V23" s="18"/>
-      <c r="W23" s="3">
+        <v>0</v>
+      </c>
+      <c r="O23" s="3">
         <v>10</v>
       </c>
-      <c r="X23" s="18"/>
-      <c r="Y23" s="3">
+      <c r="P23" s="3">
         <v>8</v>
       </c>
-      <c r="Z23" s="18"/>
-      <c r="AA23" s="18">
+      <c r="Q23" s="18">
         <v>125.717500452</v>
       </c>
-      <c r="AB23" s="18"/>
-      <c r="AC23" s="3">
+      <c r="R23" s="3">
         <v>67</v>
       </c>
-      <c r="AD23" s="15"/>
-      <c r="AE23" s="15">
+      <c r="S23" s="15">
         <v>89.706000000000003</v>
       </c>
-      <c r="AF23" s="15">
+      <c r="T23" s="15">
         <v>18.736000000000001</v>
       </c>
-      <c r="AG23" s="15"/>
-      <c r="AH23" s="10">
-        <v>50</v>
-      </c>
-      <c r="AI23" s="15"/>
-      <c r="AJ23" s="15"/>
-    </row>
-    <row r="24" spans="1:37" s="3" customFormat="1">
+    </row>
+    <row r="24" spans="1:20" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A24" s="3">
         <v>22</v>
       </c>
@@ -5773,59 +5320,44 @@
       <c r="E24" s="3">
         <v>0.3</v>
       </c>
-      <c r="H24" s="14">
+      <c r="G24" s="14">
         <v>0.30668841761827048</v>
       </c>
-      <c r="I24" s="14"/>
-      <c r="K24" s="15"/>
-      <c r="L24" s="3">
-        <v>0</v>
+      <c r="I24" s="3">
+        <v>0</v>
+      </c>
+      <c r="J24" s="3">
+        <v>0</v>
+      </c>
+      <c r="L24" s="17">
+        <v>1.5350000000000001E-2</v>
+      </c>
+      <c r="M24" s="3">
+        <v>5</v>
       </c>
       <c r="N24" s="3">
         <v>0</v>
       </c>
-      <c r="Q24" s="16"/>
-      <c r="R24" s="17">
-        <v>1.5350000000000001E-2</v>
-      </c>
-      <c r="S24" s="3">
-        <v>5</v>
-      </c>
-      <c r="T24" s="18"/>
-      <c r="U24" s="3">
-        <v>0</v>
-      </c>
-      <c r="V24" s="18"/>
-      <c r="W24" s="3">
+      <c r="O24" s="3">
         <v>4</v>
       </c>
-      <c r="X24" s="18"/>
-      <c r="Y24" s="3">
+      <c r="P24" s="3">
         <v>1</v>
       </c>
-      <c r="Z24" s="18"/>
-      <c r="AA24" s="18">
+      <c r="Q24" s="18">
         <v>124.10635293300001</v>
       </c>
-      <c r="AB24" s="18"/>
-      <c r="AC24" s="3">
+      <c r="R24" s="3">
         <v>11</v>
       </c>
-      <c r="AD24" s="15"/>
-      <c r="AE24" s="15">
+      <c r="S24" s="15">
         <v>92.912000000000006</v>
       </c>
-      <c r="AF24" s="15">
+      <c r="T24" s="15">
         <v>23.727999999999998</v>
       </c>
-      <c r="AG24" s="15"/>
-      <c r="AH24" s="10">
-        <v>50</v>
-      </c>
-      <c r="AI24" s="15"/>
-      <c r="AJ24" s="15"/>
-    </row>
-    <row r="25" spans="1:37" s="3" customFormat="1">
+    </row>
+    <row r="25" spans="1:20" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A25" s="3">
         <v>23</v>
       </c>
@@ -5841,100 +5373,69 @@
       <c r="E25" s="3">
         <v>0.25</v>
       </c>
-      <c r="H25" s="14">
+      <c r="G25" s="14">
         <v>0.20452488687782805</v>
       </c>
-      <c r="I25" s="14"/>
-      <c r="K25" s="15"/>
-      <c r="L25" s="3">
+      <c r="I25" s="3">
         <v>6</v>
       </c>
+      <c r="J25" s="3">
+        <v>1.08</v>
+      </c>
+      <c r="L25" s="17">
+        <v>6.8900000000000003E-3</v>
+      </c>
+      <c r="M25" s="3">
+        <v>14</v>
+      </c>
       <c r="N25" s="3">
-        <v>1.08</v>
-      </c>
-      <c r="Q25" s="16"/>
-      <c r="R25" s="17">
-        <v>6.8900000000000003E-3</v>
-      </c>
-      <c r="S25" s="3">
-        <v>14</v>
-      </c>
-      <c r="T25" s="18"/>
-      <c r="U25" s="3">
         <v>6</v>
       </c>
-      <c r="V25" s="18"/>
-      <c r="W25" s="3">
+      <c r="O25" s="3">
         <v>8</v>
       </c>
-      <c r="X25" s="18"/>
-      <c r="Y25" s="3">
-        <v>0</v>
-      </c>
-      <c r="Z25" s="18"/>
-      <c r="AA25" s="18">
+      <c r="P25" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q25" s="18">
         <v>145.08047818800003</v>
       </c>
-      <c r="AB25" s="18"/>
-      <c r="AC25" s="3">
+      <c r="R25" s="3">
         <v>39</v>
       </c>
-      <c r="AD25" s="15"/>
-      <c r="AE25" s="15">
+      <c r="S25" s="15">
         <v>103.84400000000001</v>
       </c>
-      <c r="AF25" s="15">
+      <c r="T25" s="15">
         <v>22.849</v>
       </c>
-      <c r="AG25" s="15"/>
-      <c r="AH25" s="10">
-        <v>50</v>
-      </c>
-      <c r="AI25" s="15"/>
-      <c r="AJ25" s="15"/>
-    </row>
-    <row r="26" spans="1:37" ht="50.45" customHeight="1">
-      <c r="D26" s="23"/>
-      <c r="E26" s="23"/>
-      <c r="J26" s="6"/>
-      <c r="K26" s="6"/>
-      <c r="L26" s="24"/>
-      <c r="M26" s="24"/>
-      <c r="N26" s="24"/>
-      <c r="O26" s="4"/>
+    </row>
+    <row r="26" spans="1:20" ht="50.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D26" s="24"/>
+      <c r="E26" s="24"/>
+      <c r="H26" s="6"/>
+      <c r="I26" s="23"/>
+      <c r="J26" s="23"/>
+      <c r="M26" s="23"/>
+      <c r="N26" s="23"/>
+      <c r="O26" s="23"/>
+      <c r="P26" s="23"/>
+      <c r="Q26" s="5"/>
+      <c r="R26" s="6"/>
       <c r="S26" s="24"/>
       <c r="T26" s="24"/>
-      <c r="U26" s="24"/>
-      <c r="V26" s="24"/>
-      <c r="W26" s="24"/>
-      <c r="X26" s="24"/>
-      <c r="Y26" s="24"/>
-      <c r="Z26" s="4"/>
-      <c r="AA26" s="5"/>
-      <c r="AB26" s="5"/>
-      <c r="AC26" s="6"/>
-      <c r="AD26" s="6"/>
-      <c r="AE26" s="23"/>
-      <c r="AF26" s="23"/>
-      <c r="AG26" s="5"/>
-      <c r="AH26" s="5"/>
-      <c r="AI26" s="5"/>
-      <c r="AJ26" s="5"/>
     </row>
   </sheetData>
-  <mergeCells count="12">
-    <mergeCell ref="S1:Y1"/>
-    <mergeCell ref="AE1:AJ1"/>
+  <mergeCells count="9">
+    <mergeCell ref="D1:H1"/>
+    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="M1:P1"/>
+    <mergeCell ref="S1:T1"/>
     <mergeCell ref="D26:E26"/>
-    <mergeCell ref="L26:N26"/>
-    <mergeCell ref="S26:Y26"/>
-    <mergeCell ref="AE26:AF26"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:K1"/>
-    <mergeCell ref="L1:N1"/>
-    <mergeCell ref="P1:R1"/>
+    <mergeCell ref="I26:J26"/>
+    <mergeCell ref="M26:P26"/>
+    <mergeCell ref="S26:T26"/>
+    <mergeCell ref="K1:L1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>

</xml_diff>